<commit_message>
Liste les carte d'un utilisateur
</commit_message>
<xml_diff>
--- a/data/Simon/Params_script.xlsx
+++ b/data/Simon/Params_script.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="30">
   <si>
     <t>Parametres</t>
   </si>
@@ -108,6 +108,12 @@
   </si>
   <si>
     <t>Ajoute un utilisateur</t>
+  </si>
+  <si>
+    <t>idUser</t>
+  </si>
+  <si>
+    <t>Liste les cartes d'un utilisateur</t>
   </si>
 </sst>
 </file>
@@ -481,10 +487,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I18"/>
+  <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -651,23 +657,23 @@
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>20</v>
+      <c r="A16" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="C16" s="1"/>
-      <c r="D16" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>11</v>
+      <c r="D16" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
       <c r="I16" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -675,7 +681,7 @@
         <v>19</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1" t="s">
@@ -687,6 +693,26 @@
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
       <c r="I18" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="I20" t="s">
         <v>27</v>
       </c>
     </row>

</xml_diff>